<commit_message>
Docs updated. Some earlier changes lost
</commit_message>
<xml_diff>
--- a/Docs/F14 PCB parts list.xlsx
+++ b/Docs/F14 PCB parts list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\MSU\Embed Sys\Lab2\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\MSU\Embed Sys\lab5\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD540E3E-F673-4D5E-A94D-5BA3CA164CCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170D4828-DF66-4F88-8297-8D45BBC70E03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="1170" windowWidth="20730" windowHeight="11775" xr2:uid="{F7341976-5CE6-4590-9369-0D7B06F7A062}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{F7341976-5CE6-4590-9369-0D7B06F7A062}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="105">
   <si>
     <t>Part Name</t>
   </si>
@@ -322,6 +322,30 @@
   </si>
   <si>
     <t>C16, 21</t>
+  </si>
+  <si>
+    <t>Newhaven Display</t>
+  </si>
+  <si>
+    <t>763-0208AZRNYBW33V</t>
+  </si>
+  <si>
+    <t>LCD Display</t>
+  </si>
+  <si>
+    <t>R6,7</t>
+  </si>
+  <si>
+    <t>470, 10K</t>
+  </si>
+  <si>
+    <t>voltage divider for contrast</t>
+  </si>
+  <si>
+    <t>LCD datasheet</t>
+  </si>
+  <si>
+    <t>2x8 chars</t>
   </si>
 </sst>
 </file>
@@ -452,7 +476,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -482,7 +506,11 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -798,16 +826,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5B82B82-34EE-4B94-980A-398253693AB3}">
-  <dimension ref="A3:G30"/>
+  <dimension ref="A3:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
     <col min="3" max="3" width="20.28515625" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="29.42578125" customWidth="1"/>
@@ -1324,48 +1352,48 @@
       <c r="F26" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G26" s="19" t="s">
+      <c r="G26" s="6" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="9">
-        <v>1</v>
-      </c>
-      <c r="E27" s="8" t="s">
+      <c r="D27" s="13">
+        <v>1</v>
+      </c>
+      <c r="E27" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F27" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="G27" s="8"/>
+      <c r="F27" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="G27" s="20"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D28" s="5">
-        <v>1</v>
-      </c>
-      <c r="E28" s="4" t="s">
+      <c r="D28" s="9">
+        <v>1</v>
+      </c>
+      <c r="E28" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="9" t="s">
         <v>55</v>
       </c>
       <c r="G28" s="2" t="s">
@@ -1393,13 +1421,48 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="4"/>
+      <c r="A30" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D30" s="5">
+        <v>1</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" s="13">
+        <v>2</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G31" s="20"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1413,8 +1476,9 @@
     <hyperlink ref="G20" r:id="rId8" xr:uid="{5C924CF4-A683-4A1C-B9C1-0DD967707A3D}"/>
     <hyperlink ref="G26" r:id="rId9" xr:uid="{1F3445A0-73CB-4481-9671-5BCC750090A9}"/>
     <hyperlink ref="G28" r:id="rId10" xr:uid="{BFF5B80F-2D9B-49F5-AF42-29EF66F727F9}"/>
+    <hyperlink ref="G30" r:id="rId11" xr:uid="{51956B82-9052-4947-A648-380AC06B26C0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>